<commit_message>
Test loading 2 samples on a single worksheet
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/double.xlsx
+++ b/storage/test_data/etl/double.xlsx
@@ -162,7 +162,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -249,8 +249,7 @@
         <v>4.42</v>
       </c>
       <c r="I2" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>116.988752455735</v>
+        <v>102.2528</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>105.1013</v>

</xml_diff>